<commit_message>
Tested test cases for iteration 9
updated bug metrics
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v2.xlsx
+++ b/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7650" tabRatio="506" firstSheet="7" activeTab="10"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7650" tabRatio="506" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 1" sheetId="3" r:id="rId1"/>
@@ -15,16 +15,17 @@
     <sheet name="Iteration 6" sheetId="9" r:id="rId6"/>
     <sheet name="Iteration 7" sheetId="10" r:id="rId7"/>
     <sheet name="Iteration 8" sheetId="13" r:id="rId8"/>
-    <sheet name="Sheet2" sheetId="11" r:id="rId9"/>
-    <sheet name="Guidelines for Bug Metrics" sheetId="2" r:id="rId10"/>
-    <sheet name="Overview" sheetId="12" r:id="rId11"/>
+    <sheet name="Iteration 9" sheetId="14" r:id="rId9"/>
+    <sheet name="Sheet2" sheetId="11" r:id="rId10"/>
+    <sheet name="Guidelines for Bug Metrics" sheetId="2" r:id="rId11"/>
+    <sheet name="Overview" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="209">
   <si>
     <t>S/N</t>
   </si>
@@ -609,6 +610,56 @@
   </si>
   <si>
     <t>https://hsemr-wpinapp.rhcloud.com/hsemr/viewPatientInformation.jsp</t>
+  </si>
+  <si>
+    <t>Iteration 7 (12 Janurary 2015-  24 Janurary 2015)</t>
+  </si>
+  <si>
+    <t>Iteration 7 (12 Janurary 2015- 24Janurary 2015)</t>
+  </si>
+  <si>
+    <t>Iteration 9 ( 9 Janurary 2015- 21 Janurary 2015)</t>
+  </si>
+  <si>
+    <t>All Case name, case description and admission information shows error when either one of the fields are empty. 
+If you empty the case description, all 3 fields will show that there is an error</t>
+  </si>
+  <si>
+    <t>http://hsemr-wpinapp.rhcloud.com/hsemr/editState.jsp</t>
+  </si>
+  <si>
+    <t>When creating a new state, healthcare provider's order field is set to be requied. However, it should be able to be left blank.</t>
+  </si>
+  <si>
+    <t>Edit state</t>
+  </si>
+  <si>
+    <t>State description can be left empty when user clicks on the save and proceed button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Case &amp; Edit Case </t>
+  </si>
+  <si>
+    <t>http://hsemr-wpinapp.rhcloud.com/hsemr/createScenario.jsp
+http://hsemr-wpinapp.rhcloud.com/hsemr/editScenario.jsp</t>
+  </si>
+  <si>
+    <t>Edit medication</t>
+  </si>
+  <si>
+    <t>under the medicine created, state information is shown instead of the medications created</t>
+  </si>
+  <si>
+    <t>Create State &amp; Edit  State</t>
+  </si>
+  <si>
+    <t>User must select discontinue state. However, the medicine might not need to be discontinued</t>
+  </si>
+  <si>
+    <t>Deactivate case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Null pointer when student is already logged in. and lecturer deactivates state. </t>
   </si>
 </sst>
 </file>
@@ -966,7 +1017,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1291,6 +1342,93 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1452,7 +1590,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1557,7 +1694,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1678,7 +1814,7 @@
                       </a:pPr>
                       <a:t>[VALUE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-SG"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1781,8 +1917,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1533781280"/>
-        <c:axId val="1533782912"/>
+        <c:axId val="171093032"/>
+        <c:axId val="176475160"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1865,7 +2001,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1929,11 +2064,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1533781280"/>
-        <c:axId val="1533782912"/>
+        <c:axId val="171093032"/>
+        <c:axId val="176475160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1533781280"/>
+        <c:axId val="171093032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1965,7 +2100,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2012,7 +2146,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1533782912"/>
+        <c:crossAx val="176475160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2020,7 +2154,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1533782912"/>
+        <c:axId val="176475160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2057,7 +2191,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1533781280"/>
+        <c:crossAx val="171093032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2071,7 +2205,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2227,7 +2360,7 @@
                       </a:pPr>
                       <a:t>[VALUE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-SG"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2330,8 +2463,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1533784000"/>
-        <c:axId val="1533776928"/>
+        <c:axId val="176475944"/>
+        <c:axId val="176476336"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2414,7 +2547,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2478,11 +2610,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1533784000"/>
-        <c:axId val="1533776928"/>
+        <c:axId val="176475944"/>
+        <c:axId val="176476336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1533784000"/>
+        <c:axId val="176475944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2514,7 +2646,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2561,7 +2692,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1533776928"/>
+        <c:crossAx val="176476336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2569,7 +2700,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1533776928"/>
+        <c:axId val="176476336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2606,7 +2737,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1533784000"/>
+        <c:crossAx val="176475944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2620,7 +2751,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3758,28 +3888,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="144" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="116"/>
-      <c r="H2" s="116"/>
-      <c r="I2" s="116"/>
-      <c r="J2" s="116"/>
-      <c r="K2" s="116"/>
-      <c r="L2" s="117"/>
+      <c r="C2" s="145"/>
+      <c r="D2" s="145"/>
+      <c r="E2" s="145"/>
+      <c r="F2" s="145"/>
+      <c r="G2" s="145"/>
+      <c r="H2" s="145"/>
+      <c r="I2" s="145"/>
+      <c r="J2" s="145"/>
+      <c r="K2" s="145"/>
+      <c r="L2" s="146"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="119" t="s">
+      <c r="B4" s="148" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="119"/>
+      <c r="C4" s="148"/>
       <c r="D4" s="15">
         <f>SUM(G8:G17)</f>
         <v>14</v>
@@ -3788,30 +3918,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="118" t="s">
+      <c r="G4" s="147" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="118"/>
-      <c r="I4" s="118"/>
-      <c r="J4" s="118"/>
-      <c r="K4" s="118"/>
-      <c r="L4" s="118"/>
+      <c r="H4" s="147"/>
+      <c r="I4" s="147"/>
+      <c r="J4" s="147"/>
+      <c r="K4" s="147"/>
+      <c r="L4" s="147"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="115" t="s">
+      <c r="B6" s="144" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="116"/>
-      <c r="D6" s="116"/>
-      <c r="E6" s="116"/>
-      <c r="F6" s="116"/>
-      <c r="G6" s="116"/>
-      <c r="H6" s="116"/>
-      <c r="I6" s="116"/>
-      <c r="J6" s="116"/>
-      <c r="K6" s="116"/>
-      <c r="L6" s="117"/>
+      <c r="C6" s="145"/>
+      <c r="D6" s="145"/>
+      <c r="E6" s="145"/>
+      <c r="F6" s="145"/>
+      <c r="G6" s="145"/>
+      <c r="H6" s="145"/>
+      <c r="I6" s="145"/>
+      <c r="J6" s="145"/>
+      <c r="K6" s="145"/>
+      <c r="L6" s="146"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="10" t="s">
@@ -4221,9 +4351,201 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="F11:O15"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="4.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="11" spans="6:15" ht="102" x14ac:dyDescent="0.25">
+      <c r="F11" s="62">
+        <v>1</v>
+      </c>
+      <c r="K11" s="63" t="s">
+        <v>129</v>
+      </c>
+      <c r="L11" s="63" t="s">
+        <v>130</v>
+      </c>
+      <c r="M11" s="64">
+        <v>41929.583333333336</v>
+      </c>
+      <c r="N11" s="65" t="s">
+        <v>131</v>
+      </c>
+      <c r="O11" s="65" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="6:15" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="F12" s="66"/>
+      <c r="G12" s="67" t="s">
+        <v>133</v>
+      </c>
+      <c r="H12" s="67" t="s">
+        <v>134</v>
+      </c>
+      <c r="I12" s="67" t="s">
+        <v>135</v>
+      </c>
+      <c r="J12" s="68">
+        <v>2</v>
+      </c>
+      <c r="K12" s="69" t="s">
+        <v>136</v>
+      </c>
+      <c r="L12" s="69" t="s">
+        <v>137</v>
+      </c>
+      <c r="M12" s="70">
+        <v>41933.475694444445</v>
+      </c>
+      <c r="N12" s="71" t="s">
+        <v>138</v>
+      </c>
+      <c r="O12" s="71" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="6:15" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="F13" s="72"/>
+      <c r="G13" s="73" t="s">
+        <v>133</v>
+      </c>
+      <c r="H13" s="73" t="s">
+        <v>134</v>
+      </c>
+      <c r="I13" s="73" t="s">
+        <v>135</v>
+      </c>
+      <c r="J13" s="74">
+        <v>3</v>
+      </c>
+      <c r="K13" s="75" t="s">
+        <v>139</v>
+      </c>
+      <c r="L13" s="75" t="s">
+        <v>140</v>
+      </c>
+      <c r="M13" s="76">
+        <v>41939.449386574073</v>
+      </c>
+      <c r="N13" s="65" t="s">
+        <v>141</v>
+      </c>
+      <c r="O13" s="65" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="6:15" ht="127.5" x14ac:dyDescent="0.25">
+      <c r="F14" s="66"/>
+      <c r="G14" s="67" t="s">
+        <v>133</v>
+      </c>
+      <c r="H14" s="67" t="s">
+        <v>134</v>
+      </c>
+      <c r="I14" s="67" t="s">
+        <v>135</v>
+      </c>
+      <c r="J14" s="68">
+        <v>4</v>
+      </c>
+      <c r="K14" s="69" t="s">
+        <v>142</v>
+      </c>
+      <c r="L14" s="69" t="s">
+        <v>143</v>
+      </c>
+      <c r="M14" s="70">
+        <v>41941.431875000002</v>
+      </c>
+      <c r="N14" s="71" t="s">
+        <v>141</v>
+      </c>
+      <c r="O14" s="71" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="6:15" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F15" s="72"/>
+      <c r="G15" s="73" t="s">
+        <v>133</v>
+      </c>
+      <c r="H15" s="73" t="s">
+        <v>134</v>
+      </c>
+      <c r="I15" s="73" t="s">
+        <v>135</v>
+      </c>
+      <c r="J15" s="74">
+        <v>5</v>
+      </c>
+      <c r="K15" s="75" t="s">
+        <v>144</v>
+      </c>
+      <c r="L15" s="75" t="s">
+        <v>145</v>
+      </c>
+      <c r="M15" s="76">
+        <v>41948.662094907406</v>
+      </c>
+      <c r="N15" s="65" t="s">
+        <v>141</v>
+      </c>
+      <c r="O15" s="65" t="s">
+        <v>146</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="N11" r:id="rId1" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=practicalgroup&amp;pos=0&amp;sql_query=SELECT+%2A+FROM+%60nphsemr%60.%60practicalgroup%60+WHERE+%60practicalGroupID%60+%3D+%27P02%27&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="O11" r:id="rId2" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=scenario&amp;pos=0&amp;sql_query=SELECT+%2A+FROM+%60nphsemr%60.%60scenario%60+WHERE+%60scenarioID%60+%3D+%27SC1%27&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="G12" r:id="rId3" display="http://localhost:55/phpmyadmin/tbl_change.php?db=nphsemr&amp;table=note&amp;where_clause=%60note%60.%60noteID%60+%3D+2&amp;clause_is_unique=1&amp;sql_query=SELECT+%2A+FROM+%60note%60&amp;goto=sql.php&amp;default_action=update&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="H12" r:id="rId4" display="http://localhost:55/phpmyadmin/tbl_change.php?db=nphsemr&amp;table=note&amp;where_clause=%60note%60.%60noteID%60+%3D+2&amp;clause_is_unique=1&amp;sql_query=SELECT+%2A+FROM+%60note%60&amp;goto=sql.php&amp;default_action=insert&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="I12" r:id="rId5" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=note&amp;sql_query=DELETE+FROM+%60nphsemr%60.%60note%60+WHERE+%60note%60.%60noteID%60+%3D+2&amp;message_to_show=The+row+has+been+deleted&amp;goto=sql.php%3Fdb%3Dnphsemr%26table%3Dnote%26sql_query%3DSELECT%2B%252A%2BFROM%2B%2560note%2560%26message_to_show%3DThe%2Brow%2Bhas%2Bbeen%2Bdeleted%26goto%3Dtbl_sql.php%26token%3Dee2d4b54d1204adf52a94b92264ae27a&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="N12" r:id="rId6" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=practicalgroup&amp;pos=0&amp;sql_query=SELECT+%2A+FROM+%60nphsemr%60.%60practicalgroup%60+WHERE+%60practicalGroupID%60+%3D+%27P03%27&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="O12" r:id="rId7" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=scenario&amp;pos=0&amp;sql_query=SELECT+%2A+FROM+%60nphsemr%60.%60scenario%60+WHERE+%60scenarioID%60+%3D+%27SC1%27&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="G13" r:id="rId8" display="http://localhost:55/phpmyadmin/tbl_change.php?db=nphsemr&amp;table=note&amp;where_clause=%60note%60.%60noteID%60+%3D+3&amp;clause_is_unique=1&amp;sql_query=SELECT+%2A+FROM+%60note%60&amp;goto=sql.php&amp;default_action=update&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="H13" r:id="rId9" display="http://localhost:55/phpmyadmin/tbl_change.php?db=nphsemr&amp;table=note&amp;where_clause=%60note%60.%60noteID%60+%3D+3&amp;clause_is_unique=1&amp;sql_query=SELECT+%2A+FROM+%60note%60&amp;goto=sql.php&amp;default_action=insert&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="I13" r:id="rId10" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=note&amp;sql_query=DELETE+FROM+%60nphsemr%60.%60note%60+WHERE+%60note%60.%60noteID%60+%3D+3&amp;message_to_show=The+row+has+been+deleted&amp;goto=sql.php%3Fdb%3Dnphsemr%26table%3Dnote%26sql_query%3DSELECT%2B%252A%2BFROM%2B%2560note%2560%26message_to_show%3DThe%2Brow%2Bhas%2Bbeen%2Bdeleted%26goto%3Dtbl_sql.php%26token%3Dee2d4b54d1204adf52a94b92264ae27a&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="N13" r:id="rId11" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=practicalgroup&amp;pos=0&amp;sql_query=SELECT+%2A+FROM+%60nphsemr%60.%60practicalgroup%60+WHERE+%60practicalGroupID%60+%3D+%27P01%27&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="O13" r:id="rId12" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=scenario&amp;pos=0&amp;sql_query=SELECT+%2A+FROM+%60nphsemr%60.%60scenario%60+WHERE+%60scenarioID%60+%3D+%27SC1%27&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="G14" r:id="rId13" display="http://localhost:55/phpmyadmin/tbl_change.php?db=nphsemr&amp;table=note&amp;where_clause=%60note%60.%60noteID%60+%3D+4&amp;clause_is_unique=1&amp;sql_query=SELECT+%2A+FROM+%60note%60&amp;goto=sql.php&amp;default_action=update&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="H14" r:id="rId14" display="http://localhost:55/phpmyadmin/tbl_change.php?db=nphsemr&amp;table=note&amp;where_clause=%60note%60.%60noteID%60+%3D+4&amp;clause_is_unique=1&amp;sql_query=SELECT+%2A+FROM+%60note%60&amp;goto=sql.php&amp;default_action=insert&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="I14" r:id="rId15" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=note&amp;sql_query=DELETE+FROM+%60nphsemr%60.%60note%60+WHERE+%60note%60.%60noteID%60+%3D+4&amp;message_to_show=The+row+has+been+deleted&amp;goto=sql.php%3Fdb%3Dnphsemr%26table%3Dnote%26sql_query%3DSELECT%2B%252A%2BFROM%2B%2560note%2560%26message_to_show%3DThe%2Brow%2Bhas%2Bbeen%2Bdeleted%26goto%3Dtbl_sql.php%26token%3Dee2d4b54d1204adf52a94b92264ae27a&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="N14" r:id="rId16" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=practicalgroup&amp;pos=0&amp;sql_query=SELECT+%2A+FROM+%60nphsemr%60.%60practicalgroup%60+WHERE+%60practicalGroupID%60+%3D+%27P01%27&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="O14" r:id="rId17" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=scenario&amp;pos=0&amp;sql_query=SELECT+%2A+FROM+%60nphsemr%60.%60scenario%60+WHERE+%60scenarioID%60+%3D+%27SC1%27&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="G15" r:id="rId18" display="http://localhost:55/phpmyadmin/tbl_change.php?db=nphsemr&amp;table=note&amp;where_clause=%60note%60.%60noteID%60+%3D+5&amp;clause_is_unique=1&amp;sql_query=SELECT+%2A+FROM+%60note%60&amp;goto=sql.php&amp;default_action=update&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="H15" r:id="rId19" display="http://localhost:55/phpmyadmin/tbl_change.php?db=nphsemr&amp;table=note&amp;where_clause=%60note%60.%60noteID%60+%3D+5&amp;clause_is_unique=1&amp;sql_query=SELECT+%2A+FROM+%60note%60&amp;goto=sql.php&amp;default_action=insert&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="I15" r:id="rId20" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=note&amp;sql_query=DELETE+FROM+%60nphsemr%60.%60note%60+WHERE+%60note%60.%60noteID%60+%3D+5&amp;message_to_show=The+row+has+been+deleted&amp;goto=sql.php%3Fdb%3Dnphsemr%26table%3Dnote%26sql_query%3DSELECT%2B%252A%2BFROM%2B%2560note%2560%26message_to_show%3DThe%2Brow%2Bhas%2Bbeen%2Bdeleted%26goto%3Dtbl_sql.php%26token%3Dee2d4b54d1204adf52a94b92264ae27a&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="N15" r:id="rId21" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=practicalgroup&amp;pos=0&amp;sql_query=SELECT+%2A+FROM+%60nphsemr%60.%60practicalgroup%60+WHERE+%60practicalGroupID%60+%3D+%27P01%27&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="O15" r:id="rId22" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=scenario&amp;pos=0&amp;sql_query=SELECT+%2A+FROM+%60nphsemr%60.%60scenario%60+WHERE+%60scenarioID%60+%3D+%27SC4%27&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId23"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -4367,11 +4689,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="W23" sqref="W23"/>
     </sheetView>
   </sheetViews>
@@ -4558,28 +4880,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="144" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="116"/>
-      <c r="H2" s="116"/>
-      <c r="I2" s="116"/>
-      <c r="J2" s="116"/>
-      <c r="K2" s="116"/>
-      <c r="L2" s="117"/>
+      <c r="C2" s="145"/>
+      <c r="D2" s="145"/>
+      <c r="E2" s="145"/>
+      <c r="F2" s="145"/>
+      <c r="G2" s="145"/>
+      <c r="H2" s="145"/>
+      <c r="I2" s="145"/>
+      <c r="J2" s="145"/>
+      <c r="K2" s="145"/>
+      <c r="L2" s="146"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="119" t="s">
+      <c r="B4" s="148" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="119"/>
+      <c r="C4" s="148"/>
       <c r="D4" s="15">
         <f>SUM(G8:G10)</f>
         <v>11</v>
@@ -4588,30 +4910,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="118" t="s">
+      <c r="G4" s="147" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="118"/>
-      <c r="I4" s="118"/>
-      <c r="J4" s="118"/>
-      <c r="K4" s="118"/>
-      <c r="L4" s="118"/>
+      <c r="H4" s="147"/>
+      <c r="I4" s="147"/>
+      <c r="J4" s="147"/>
+      <c r="K4" s="147"/>
+      <c r="L4" s="147"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="115" t="s">
+      <c r="B6" s="144" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="116"/>
-      <c r="D6" s="116"/>
-      <c r="E6" s="116"/>
-      <c r="F6" s="116"/>
-      <c r="G6" s="116"/>
-      <c r="H6" s="116"/>
-      <c r="I6" s="116"/>
-      <c r="J6" s="116"/>
-      <c r="K6" s="116"/>
-      <c r="L6" s="117"/>
+      <c r="C6" s="145"/>
+      <c r="D6" s="145"/>
+      <c r="E6" s="145"/>
+      <c r="F6" s="145"/>
+      <c r="G6" s="145"/>
+      <c r="H6" s="145"/>
+      <c r="I6" s="145"/>
+      <c r="J6" s="145"/>
+      <c r="K6" s="145"/>
+      <c r="L6" s="146"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="17" t="s">
@@ -4908,28 +5230,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="144" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="116"/>
-      <c r="H2" s="116"/>
-      <c r="I2" s="116"/>
-      <c r="J2" s="116"/>
-      <c r="K2" s="116"/>
-      <c r="L2" s="117"/>
+      <c r="C2" s="145"/>
+      <c r="D2" s="145"/>
+      <c r="E2" s="145"/>
+      <c r="F2" s="145"/>
+      <c r="G2" s="145"/>
+      <c r="H2" s="145"/>
+      <c r="I2" s="145"/>
+      <c r="J2" s="145"/>
+      <c r="K2" s="145"/>
+      <c r="L2" s="146"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="119" t="s">
+      <c r="B4" s="148" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="119"/>
+      <c r="C4" s="148"/>
       <c r="D4" s="22">
         <f>SUM(G8:G10)</f>
         <v>15</v>
@@ -4938,30 +5260,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="118" t="s">
+      <c r="G4" s="147" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="118"/>
-      <c r="I4" s="118"/>
-      <c r="J4" s="118"/>
-      <c r="K4" s="118"/>
-      <c r="L4" s="118"/>
+      <c r="H4" s="147"/>
+      <c r="I4" s="147"/>
+      <c r="J4" s="147"/>
+      <c r="K4" s="147"/>
+      <c r="L4" s="147"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="115" t="s">
+      <c r="B6" s="144" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="116"/>
-      <c r="D6" s="116"/>
-      <c r="E6" s="116"/>
-      <c r="F6" s="116"/>
-      <c r="G6" s="116"/>
-      <c r="H6" s="116"/>
-      <c r="I6" s="116"/>
-      <c r="J6" s="116"/>
-      <c r="K6" s="116"/>
-      <c r="L6" s="117"/>
+      <c r="C6" s="145"/>
+      <c r="D6" s="145"/>
+      <c r="E6" s="145"/>
+      <c r="F6" s="145"/>
+      <c r="G6" s="145"/>
+      <c r="H6" s="145"/>
+      <c r="I6" s="145"/>
+      <c r="J6" s="145"/>
+      <c r="K6" s="145"/>
+      <c r="L6" s="146"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="27" t="s">
@@ -5259,28 +5581,28 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="120" t="s">
+      <c r="B2" s="149" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="121"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="121"/>
-      <c r="F2" s="121"/>
-      <c r="G2" s="121"/>
-      <c r="H2" s="121"/>
-      <c r="I2" s="121"/>
-      <c r="J2" s="121"/>
-      <c r="K2" s="121"/>
-      <c r="L2" s="122"/>
+      <c r="C2" s="150"/>
+      <c r="D2" s="150"/>
+      <c r="E2" s="150"/>
+      <c r="F2" s="150"/>
+      <c r="G2" s="150"/>
+      <c r="H2" s="150"/>
+      <c r="I2" s="150"/>
+      <c r="J2" s="150"/>
+      <c r="K2" s="150"/>
+      <c r="L2" s="151"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="123" t="s">
+      <c r="B4" s="152" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="124"/>
+      <c r="C4" s="153"/>
       <c r="D4" s="22">
         <f>SUM(G8:G10)</f>
         <v>5</v>
@@ -5289,30 +5611,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="125" t="s">
+      <c r="G4" s="154" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="126"/>
-      <c r="I4" s="126"/>
-      <c r="J4" s="126"/>
-      <c r="K4" s="126"/>
-      <c r="L4" s="127"/>
+      <c r="H4" s="155"/>
+      <c r="I4" s="155"/>
+      <c r="J4" s="155"/>
+      <c r="K4" s="155"/>
+      <c r="L4" s="156"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="120" t="s">
+      <c r="B6" s="149" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="121"/>
-      <c r="D6" s="121"/>
-      <c r="E6" s="121"/>
-      <c r="F6" s="121"/>
-      <c r="G6" s="121"/>
-      <c r="H6" s="121"/>
-      <c r="I6" s="121"/>
-      <c r="J6" s="121"/>
-      <c r="K6" s="121"/>
-      <c r="L6" s="122"/>
+      <c r="C6" s="150"/>
+      <c r="D6" s="150"/>
+      <c r="E6" s="150"/>
+      <c r="F6" s="150"/>
+      <c r="G6" s="150"/>
+      <c r="H6" s="150"/>
+      <c r="I6" s="150"/>
+      <c r="J6" s="150"/>
+      <c r="K6" s="150"/>
+      <c r="L6" s="151"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="33" t="s">
@@ -5604,28 +5926,28 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="120" t="s">
+      <c r="B2" s="149" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="121"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="121"/>
-      <c r="F2" s="121"/>
-      <c r="G2" s="121"/>
-      <c r="H2" s="121"/>
-      <c r="I2" s="121"/>
-      <c r="J2" s="121"/>
-      <c r="K2" s="121"/>
-      <c r="L2" s="122"/>
+      <c r="C2" s="150"/>
+      <c r="D2" s="150"/>
+      <c r="E2" s="150"/>
+      <c r="F2" s="150"/>
+      <c r="G2" s="150"/>
+      <c r="H2" s="150"/>
+      <c r="I2" s="150"/>
+      <c r="J2" s="150"/>
+      <c r="K2" s="150"/>
+      <c r="L2" s="151"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="123" t="s">
+      <c r="B4" s="152" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="124"/>
+      <c r="C4" s="153"/>
       <c r="D4" s="22">
         <f>SUM(G8:G116)</f>
         <v>30</v>
@@ -5634,30 +5956,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="125" t="s">
+      <c r="G4" s="154" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="126"/>
-      <c r="I4" s="126"/>
-      <c r="J4" s="126"/>
-      <c r="K4" s="126"/>
-      <c r="L4" s="127"/>
+      <c r="H4" s="155"/>
+      <c r="I4" s="155"/>
+      <c r="J4" s="155"/>
+      <c r="K4" s="155"/>
+      <c r="L4" s="156"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="120" t="s">
+      <c r="B6" s="149" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="121"/>
-      <c r="D6" s="121"/>
-      <c r="E6" s="121"/>
-      <c r="F6" s="121"/>
-      <c r="G6" s="121"/>
-      <c r="H6" s="121"/>
-      <c r="I6" s="121"/>
-      <c r="J6" s="121"/>
-      <c r="K6" s="121"/>
-      <c r="L6" s="122"/>
+      <c r="C6" s="150"/>
+      <c r="D6" s="150"/>
+      <c r="E6" s="150"/>
+      <c r="F6" s="150"/>
+      <c r="G6" s="150"/>
+      <c r="H6" s="150"/>
+      <c r="I6" s="150"/>
+      <c r="J6" s="150"/>
+      <c r="K6" s="150"/>
+      <c r="L6" s="151"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="41" t="s">
@@ -6050,26 +6372,26 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="128" t="s">
+      <c r="B2" s="157" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="129"/>
-      <c r="D2" s="129"/>
-      <c r="E2" s="129"/>
-      <c r="F2" s="129"/>
-      <c r="G2" s="129"/>
-      <c r="H2" s="129"/>
-      <c r="I2" s="129"/>
-      <c r="J2" s="129"/>
-      <c r="K2" s="129"/>
-      <c r="L2" s="130"/>
+      <c r="C2" s="158"/>
+      <c r="D2" s="158"/>
+      <c r="E2" s="158"/>
+      <c r="F2" s="158"/>
+      <c r="G2" s="158"/>
+      <c r="H2" s="158"/>
+      <c r="I2" s="158"/>
+      <c r="J2" s="158"/>
+      <c r="K2" s="158"/>
+      <c r="L2" s="159"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="131" t="s">
+      <c r="B4" s="160" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="132"/>
+      <c r="C4" s="161"/>
       <c r="D4" s="44">
         <f>SUM(G8:G116)</f>
         <v>20</v>
@@ -6078,30 +6400,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="125" t="s">
+      <c r="G4" s="154" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="126"/>
-      <c r="I4" s="126"/>
-      <c r="J4" s="126"/>
-      <c r="K4" s="126"/>
-      <c r="L4" s="127"/>
+      <c r="H4" s="155"/>
+      <c r="I4" s="155"/>
+      <c r="J4" s="155"/>
+      <c r="K4" s="155"/>
+      <c r="L4" s="156"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="128" t="s">
+      <c r="B6" s="157" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="129"/>
-      <c r="D6" s="129"/>
-      <c r="E6" s="129"/>
-      <c r="F6" s="129"/>
-      <c r="G6" s="129"/>
-      <c r="H6" s="129"/>
-      <c r="I6" s="129"/>
-      <c r="J6" s="129"/>
-      <c r="K6" s="129"/>
-      <c r="L6" s="130"/>
+      <c r="C6" s="158"/>
+      <c r="D6" s="158"/>
+      <c r="E6" s="158"/>
+      <c r="F6" s="158"/>
+      <c r="G6" s="158"/>
+      <c r="H6" s="158"/>
+      <c r="I6" s="158"/>
+      <c r="J6" s="158"/>
+      <c r="K6" s="158"/>
+      <c r="L6" s="159"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="34" t="s">
@@ -6438,8 +6760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6462,26 +6784,26 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="128" t="s">
-        <v>116</v>
-      </c>
-      <c r="C2" s="129"/>
-      <c r="D2" s="129"/>
-      <c r="E2" s="129"/>
-      <c r="F2" s="129"/>
-      <c r="G2" s="129"/>
-      <c r="H2" s="129"/>
-      <c r="I2" s="129"/>
-      <c r="J2" s="129"/>
-      <c r="K2" s="129"/>
-      <c r="L2" s="130"/>
+      <c r="B2" s="157" t="s">
+        <v>193</v>
+      </c>
+      <c r="C2" s="158"/>
+      <c r="D2" s="158"/>
+      <c r="E2" s="158"/>
+      <c r="F2" s="158"/>
+      <c r="G2" s="158"/>
+      <c r="H2" s="158"/>
+      <c r="I2" s="158"/>
+      <c r="J2" s="158"/>
+      <c r="K2" s="158"/>
+      <c r="L2" s="159"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="131" t="s">
+      <c r="B4" s="160" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="132"/>
+      <c r="C4" s="161"/>
       <c r="D4" s="44">
         <f>SUM(G8:G116)</f>
         <v>20</v>
@@ -6490,30 +6812,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="125" t="s">
+      <c r="G4" s="154" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="126"/>
-      <c r="I4" s="126"/>
-      <c r="J4" s="126"/>
-      <c r="K4" s="126"/>
-      <c r="L4" s="127"/>
+      <c r="H4" s="155"/>
+      <c r="I4" s="155"/>
+      <c r="J4" s="155"/>
+      <c r="K4" s="155"/>
+      <c r="L4" s="156"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="128" t="s">
-        <v>116</v>
-      </c>
-      <c r="C6" s="129"/>
-      <c r="D6" s="129"/>
-      <c r="E6" s="129"/>
-      <c r="F6" s="129"/>
-      <c r="G6" s="129"/>
-      <c r="H6" s="129"/>
-      <c r="I6" s="129"/>
-      <c r="J6" s="129"/>
-      <c r="K6" s="129"/>
-      <c r="L6" s="130"/>
+      <c r="B6" s="157" t="s">
+        <v>194</v>
+      </c>
+      <c r="C6" s="158"/>
+      <c r="D6" s="158"/>
+      <c r="E6" s="158"/>
+      <c r="F6" s="158"/>
+      <c r="G6" s="158"/>
+      <c r="H6" s="158"/>
+      <c r="I6" s="158"/>
+      <c r="J6" s="158"/>
+      <c r="K6" s="158"/>
+      <c r="L6" s="159"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="78" t="s">
@@ -6964,7 +7286,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
@@ -6988,26 +7310,26 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="128" t="s">
+      <c r="B2" s="157" t="s">
         <v>164</v>
       </c>
-      <c r="C2" s="129"/>
-      <c r="D2" s="129"/>
-      <c r="E2" s="129"/>
-      <c r="F2" s="129"/>
-      <c r="G2" s="129"/>
-      <c r="H2" s="129"/>
-      <c r="I2" s="129"/>
-      <c r="J2" s="129"/>
-      <c r="K2" s="129"/>
-      <c r="L2" s="130"/>
+      <c r="C2" s="158"/>
+      <c r="D2" s="158"/>
+      <c r="E2" s="158"/>
+      <c r="F2" s="158"/>
+      <c r="G2" s="158"/>
+      <c r="H2" s="158"/>
+      <c r="I2" s="158"/>
+      <c r="J2" s="158"/>
+      <c r="K2" s="158"/>
+      <c r="L2" s="159"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="131" t="s">
+      <c r="B4" s="160" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="132"/>
+      <c r="C4" s="161"/>
       <c r="D4" s="44">
         <f>SUM(G8:G110)</f>
         <v>32</v>
@@ -7016,30 +7338,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="125" t="s">
+      <c r="G4" s="154" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="126"/>
-      <c r="I4" s="126"/>
-      <c r="J4" s="126"/>
-      <c r="K4" s="126"/>
-      <c r="L4" s="127"/>
+      <c r="H4" s="155"/>
+      <c r="I4" s="155"/>
+      <c r="J4" s="155"/>
+      <c r="K4" s="155"/>
+      <c r="L4" s="156"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="128" t="s">
+      <c r="B6" s="157" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="129"/>
-      <c r="D6" s="129"/>
-      <c r="E6" s="129"/>
-      <c r="F6" s="129"/>
-      <c r="G6" s="129"/>
-      <c r="H6" s="129"/>
-      <c r="I6" s="129"/>
-      <c r="J6" s="129"/>
-      <c r="K6" s="129"/>
-      <c r="L6" s="130"/>
+      <c r="C6" s="158"/>
+      <c r="D6" s="158"/>
+      <c r="E6" s="158"/>
+      <c r="F6" s="158"/>
+      <c r="G6" s="158"/>
+      <c r="H6" s="158"/>
+      <c r="I6" s="158"/>
+      <c r="J6" s="158"/>
+      <c r="K6" s="158"/>
+      <c r="L6" s="159"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="110" t="s">
@@ -7426,192 +7748,416 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="F11:O15"/>
+  <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="43"/>
+    <col min="2" max="2" width="4.42578125" style="43" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" style="43" customWidth="1"/>
+    <col min="4" max="4" width="42.5703125" style="43" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="43" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="43" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" style="43" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" style="43" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="43" customWidth="1"/>
+    <col min="10" max="10" width="31" style="43" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" style="43" customWidth="1"/>
+    <col min="12" max="12" width="14" style="43" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" style="43" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="43"/>
   </cols>
   <sheetData>
-    <row r="11" spans="6:15" ht="102" x14ac:dyDescent="0.25">
-      <c r="F11" s="62">
+    <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="157" t="s">
+        <v>195</v>
+      </c>
+      <c r="C2" s="158"/>
+      <c r="D2" s="158"/>
+      <c r="E2" s="158"/>
+      <c r="F2" s="158"/>
+      <c r="G2" s="158"/>
+      <c r="H2" s="158"/>
+      <c r="I2" s="158"/>
+      <c r="J2" s="158"/>
+      <c r="K2" s="158"/>
+      <c r="L2" s="159"/>
+    </row>
+    <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="160" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="161"/>
+      <c r="D4" s="44">
+        <f>SUM(G8:G116)</f>
+        <v>26</v>
+      </c>
+      <c r="E4" s="45"/>
+      <c r="F4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="154"/>
+      <c r="H4" s="155"/>
+      <c r="I4" s="155"/>
+      <c r="J4" s="155"/>
+      <c r="K4" s="155"/>
+      <c r="L4" s="156"/>
+    </row>
+    <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="157" t="s">
+        <v>195</v>
+      </c>
+      <c r="C6" s="158"/>
+      <c r="D6" s="158"/>
+      <c r="E6" s="158"/>
+      <c r="F6" s="158"/>
+      <c r="G6" s="158"/>
+      <c r="H6" s="158"/>
+      <c r="I6" s="158"/>
+      <c r="J6" s="158"/>
+      <c r="K6" s="158"/>
+      <c r="L6" s="159"/>
+    </row>
+    <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="115" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="K11" s="63" t="s">
-        <v>129</v>
-      </c>
-      <c r="L11" s="63" t="s">
-        <v>130</v>
-      </c>
-      <c r="M11" s="64">
-        <v>41929.583333333336</v>
-      </c>
-      <c r="N11" s="65" t="s">
-        <v>131</v>
-      </c>
-      <c r="O11" s="65" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="12" spans="6:15" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="F12" s="66"/>
-      <c r="G12" s="67" t="s">
-        <v>133</v>
-      </c>
-      <c r="H12" s="67" t="s">
-        <v>134</v>
-      </c>
-      <c r="I12" s="67" t="s">
-        <v>135</v>
-      </c>
-      <c r="J12" s="68">
+      <c r="D7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="115" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="K12" s="69" t="s">
-        <v>136</v>
-      </c>
-      <c r="L12" s="69" t="s">
-        <v>137</v>
-      </c>
-      <c r="M12" s="70">
-        <v>41933.475694444445</v>
-      </c>
-      <c r="N12" s="71" t="s">
-        <v>138</v>
-      </c>
-      <c r="O12" s="71" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="13" spans="6:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="F13" s="72"/>
-      <c r="G13" s="73" t="s">
-        <v>133</v>
-      </c>
-      <c r="H13" s="73" t="s">
-        <v>134</v>
-      </c>
-      <c r="I13" s="73" t="s">
-        <v>135</v>
-      </c>
-      <c r="J13" s="74">
+      <c r="G7" s="115" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="115" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="115" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="K13" s="75" t="s">
-        <v>139</v>
-      </c>
-      <c r="L13" s="75" t="s">
-        <v>140</v>
-      </c>
-      <c r="M13" s="76">
-        <v>41939.449386574073</v>
-      </c>
-      <c r="N13" s="65" t="s">
-        <v>141</v>
-      </c>
-      <c r="O13" s="65" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="14" spans="6:15" ht="127.5" x14ac:dyDescent="0.25">
-      <c r="F14" s="66"/>
-      <c r="G14" s="67" t="s">
-        <v>133</v>
-      </c>
-      <c r="H14" s="67" t="s">
-        <v>134</v>
-      </c>
-      <c r="I14" s="67" t="s">
-        <v>135</v>
-      </c>
-      <c r="J14" s="68">
+    </row>
+    <row r="8" spans="1:17" ht="165.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="30">
+        <v>1</v>
+      </c>
+      <c r="C8" s="141" t="s">
+        <v>201</v>
+      </c>
+      <c r="D8" s="139" t="s">
+        <v>202</v>
+      </c>
+      <c r="E8" s="140" t="s">
+        <v>196</v>
+      </c>
+      <c r="F8" s="116">
+        <v>42050</v>
+      </c>
+      <c r="G8" s="118">
+        <v>5</v>
+      </c>
+      <c r="H8" s="118"/>
+      <c r="I8" s="119"/>
+      <c r="J8" s="119"/>
+      <c r="K8" s="120"/>
+      <c r="L8" s="121"/>
+    </row>
+    <row r="9" spans="1:17" ht="81.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="46"/>
+      <c r="B9" s="83">
+        <v>2</v>
+      </c>
+      <c r="C9" s="143" t="s">
+        <v>205</v>
+      </c>
+      <c r="D9" s="142" t="s">
+        <v>197</v>
+      </c>
+      <c r="E9" s="116" t="s">
+        <v>198</v>
+      </c>
+      <c r="F9" s="116">
+        <v>42050</v>
+      </c>
+      <c r="G9" s="118">
+        <v>1</v>
+      </c>
+      <c r="H9" s="118"/>
+      <c r="I9" s="119"/>
+      <c r="J9" s="119"/>
+      <c r="K9" s="123"/>
+      <c r="L9" s="121"/>
+      <c r="M9" s="46"/>
+      <c r="N9" s="46"/>
+      <c r="O9" s="46"/>
+      <c r="P9" s="46"/>
+      <c r="Q9" s="46"/>
+    </row>
+    <row r="10" spans="1:17" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="46"/>
+      <c r="B10" s="83">
+        <v>3</v>
+      </c>
+      <c r="C10" s="119" t="s">
+        <v>199</v>
+      </c>
+      <c r="D10" s="122" t="s">
+        <v>197</v>
+      </c>
+      <c r="E10" s="124" t="s">
+        <v>200</v>
+      </c>
+      <c r="F10" s="116">
+        <v>42050</v>
+      </c>
+      <c r="G10" s="118">
+        <v>5</v>
+      </c>
+      <c r="H10" s="125"/>
+      <c r="I10" s="121"/>
+      <c r="J10" s="121"/>
+      <c r="K10" s="121"/>
+      <c r="L10" s="121"/>
+      <c r="M10" s="46"/>
+      <c r="N10" s="46"/>
+      <c r="O10" s="46"/>
+      <c r="P10" s="46"/>
+      <c r="Q10" s="46"/>
+    </row>
+    <row r="11" spans="1:17" ht="68.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="46"/>
+      <c r="B11" s="30">
         <v>4</v>
       </c>
-      <c r="K14" s="69" t="s">
-        <v>142</v>
-      </c>
-      <c r="L14" s="69" t="s">
-        <v>143</v>
-      </c>
-      <c r="M14" s="70">
-        <v>41941.431875000002</v>
-      </c>
-      <c r="N14" s="71" t="s">
-        <v>141</v>
-      </c>
-      <c r="O14" s="71" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="15" spans="6:15" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="F15" s="72"/>
-      <c r="G15" s="73" t="s">
-        <v>133</v>
-      </c>
-      <c r="H15" s="73" t="s">
-        <v>134</v>
-      </c>
-      <c r="I15" s="73" t="s">
-        <v>135</v>
-      </c>
-      <c r="J15" s="74">
+      <c r="C11" s="126" t="s">
+        <v>203</v>
+      </c>
+      <c r="D11" s="117" t="s">
+        <v>151</v>
+      </c>
+      <c r="E11" s="119" t="s">
+        <v>204</v>
+      </c>
+      <c r="F11" s="116">
+        <v>42050</v>
+      </c>
+      <c r="G11" s="119">
         <v>5</v>
       </c>
-      <c r="K15" s="75" t="s">
-        <v>144</v>
-      </c>
-      <c r="L15" s="75" t="s">
-        <v>145</v>
-      </c>
-      <c r="M15" s="76">
-        <v>41948.662094907406</v>
-      </c>
-      <c r="N15" s="65" t="s">
-        <v>141</v>
-      </c>
-      <c r="O15" s="65" t="s">
-        <v>146</v>
-      </c>
+      <c r="H11" s="127"/>
+      <c r="I11" s="119"/>
+      <c r="J11" s="123"/>
+      <c r="K11" s="123"/>
+      <c r="L11" s="123"/>
+      <c r="M11" s="46"/>
+      <c r="N11" s="46"/>
+      <c r="O11" s="46"/>
+      <c r="P11" s="46"/>
+      <c r="Q11" s="46"/>
+    </row>
+    <row r="12" spans="1:17" ht="68.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="46"/>
+      <c r="B12" s="85">
+        <v>5</v>
+      </c>
+      <c r="C12" s="126" t="s">
+        <v>201</v>
+      </c>
+      <c r="D12" s="117" t="s">
+        <v>151</v>
+      </c>
+      <c r="E12" s="119" t="s">
+        <v>206</v>
+      </c>
+      <c r="F12" s="116">
+        <v>42050</v>
+      </c>
+      <c r="G12" s="119">
+        <v>5</v>
+      </c>
+      <c r="H12" s="120"/>
+      <c r="I12" s="119"/>
+      <c r="J12" s="128"/>
+      <c r="K12" s="129"/>
+      <c r="L12" s="121"/>
+      <c r="M12" s="46"/>
+      <c r="N12" s="46"/>
+      <c r="O12" s="46"/>
+      <c r="P12" s="46"/>
+      <c r="Q12" s="46"/>
+    </row>
+    <row r="13" spans="1:17" ht="50.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="77"/>
+      <c r="B13" s="87">
+        <v>6</v>
+      </c>
+      <c r="C13" s="130" t="s">
+        <v>207</v>
+      </c>
+      <c r="D13" s="131" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="132" t="s">
+        <v>208</v>
+      </c>
+      <c r="F13" s="116">
+        <v>42050</v>
+      </c>
+      <c r="G13" s="133">
+        <v>5</v>
+      </c>
+      <c r="H13" s="134"/>
+      <c r="I13" s="133"/>
+      <c r="J13" s="98"/>
+      <c r="K13" s="132"/>
+      <c r="L13" s="135"/>
+      <c r="M13" s="77"/>
+      <c r="N13" s="77"/>
+      <c r="O13" s="77"/>
+      <c r="P13" s="77"/>
+      <c r="Q13" s="77"/>
+    </row>
+    <row r="14" spans="1:17" s="79" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="80"/>
+      <c r="B14" s="89">
+        <v>7</v>
+      </c>
+      <c r="C14" s="129"/>
+      <c r="D14" s="136"/>
+      <c r="E14" s="129"/>
+      <c r="F14" s="116"/>
+      <c r="G14" s="129"/>
+      <c r="H14" s="134"/>
+      <c r="I14" s="129"/>
+      <c r="J14" s="129"/>
+      <c r="K14" s="129"/>
+      <c r="L14" s="121"/>
+      <c r="M14" s="80"/>
+      <c r="N14" s="80"/>
+      <c r="O14" s="80"/>
+      <c r="P14" s="80"/>
+      <c r="Q14" s="80"/>
+    </row>
+    <row r="15" spans="1:17" s="79" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="80"/>
+      <c r="B15" s="92">
+        <v>8</v>
+      </c>
+      <c r="C15" s="129"/>
+      <c r="D15" s="131"/>
+      <c r="E15" s="138"/>
+      <c r="F15" s="137"/>
+      <c r="G15" s="138"/>
+      <c r="H15" s="133"/>
+      <c r="I15" s="138"/>
+      <c r="J15" s="138"/>
+      <c r="K15" s="138"/>
+      <c r="L15" s="121"/>
+      <c r="M15" s="80"/>
+      <c r="N15" s="80"/>
+      <c r="O15" s="80"/>
+      <c r="P15" s="80"/>
+      <c r="Q15" s="80"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B16" s="46"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="51" t="str">
+        <f>IFERROR(VLOOKUP(G16,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v/>
+      </c>
+      <c r="I16" s="46"/>
+      <c r="J16" s="46"/>
+      <c r="K16" s="46"/>
+      <c r="L16" s="46"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B17" s="46"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="51" t="str">
+        <f>IFERROR(VLOOKUP(G17,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v/>
+      </c>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="46"/>
+      <c r="L17" s="46"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="H18" s="51" t="str">
+        <f>IFERROR(VLOOKUP(G18,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="H19" s="51" t="str">
+        <f>IFERROR(VLOOKUP(G19,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="H20" s="51" t="str">
+        <f>IFERROR(VLOOKUP(G20,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="H21" s="51" t="str">
+        <f>IFERROR(VLOOKUP(G21,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="H22" s="49"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="H23" s="49"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="H24" s="49"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="G4:L4"/>
+    <mergeCell ref="B6:L6"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="N11" r:id="rId1" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=practicalgroup&amp;pos=0&amp;sql_query=SELECT+%2A+FROM+%60nphsemr%60.%60practicalgroup%60+WHERE+%60practicalGroupID%60+%3D+%27P02%27&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
-    <hyperlink ref="O11" r:id="rId2" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=scenario&amp;pos=0&amp;sql_query=SELECT+%2A+FROM+%60nphsemr%60.%60scenario%60+WHERE+%60scenarioID%60+%3D+%27SC1%27&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
-    <hyperlink ref="G12" r:id="rId3" display="http://localhost:55/phpmyadmin/tbl_change.php?db=nphsemr&amp;table=note&amp;where_clause=%60note%60.%60noteID%60+%3D+2&amp;clause_is_unique=1&amp;sql_query=SELECT+%2A+FROM+%60note%60&amp;goto=sql.php&amp;default_action=update&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
-    <hyperlink ref="H12" r:id="rId4" display="http://localhost:55/phpmyadmin/tbl_change.php?db=nphsemr&amp;table=note&amp;where_clause=%60note%60.%60noteID%60+%3D+2&amp;clause_is_unique=1&amp;sql_query=SELECT+%2A+FROM+%60note%60&amp;goto=sql.php&amp;default_action=insert&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
-    <hyperlink ref="I12" r:id="rId5" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=note&amp;sql_query=DELETE+FROM+%60nphsemr%60.%60note%60+WHERE+%60note%60.%60noteID%60+%3D+2&amp;message_to_show=The+row+has+been+deleted&amp;goto=sql.php%3Fdb%3Dnphsemr%26table%3Dnote%26sql_query%3DSELECT%2B%252A%2BFROM%2B%2560note%2560%26message_to_show%3DThe%2Brow%2Bhas%2Bbeen%2Bdeleted%26goto%3Dtbl_sql.php%26token%3Dee2d4b54d1204adf52a94b92264ae27a&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
-    <hyperlink ref="N12" r:id="rId6" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=practicalgroup&amp;pos=0&amp;sql_query=SELECT+%2A+FROM+%60nphsemr%60.%60practicalgroup%60+WHERE+%60practicalGroupID%60+%3D+%27P03%27&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
-    <hyperlink ref="O12" r:id="rId7" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=scenario&amp;pos=0&amp;sql_query=SELECT+%2A+FROM+%60nphsemr%60.%60scenario%60+WHERE+%60scenarioID%60+%3D+%27SC1%27&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
-    <hyperlink ref="G13" r:id="rId8" display="http://localhost:55/phpmyadmin/tbl_change.php?db=nphsemr&amp;table=note&amp;where_clause=%60note%60.%60noteID%60+%3D+3&amp;clause_is_unique=1&amp;sql_query=SELECT+%2A+FROM+%60note%60&amp;goto=sql.php&amp;default_action=update&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
-    <hyperlink ref="H13" r:id="rId9" display="http://localhost:55/phpmyadmin/tbl_change.php?db=nphsemr&amp;table=note&amp;where_clause=%60note%60.%60noteID%60+%3D+3&amp;clause_is_unique=1&amp;sql_query=SELECT+%2A+FROM+%60note%60&amp;goto=sql.php&amp;default_action=insert&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
-    <hyperlink ref="I13" r:id="rId10" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=note&amp;sql_query=DELETE+FROM+%60nphsemr%60.%60note%60+WHERE+%60note%60.%60noteID%60+%3D+3&amp;message_to_show=The+row+has+been+deleted&amp;goto=sql.php%3Fdb%3Dnphsemr%26table%3Dnote%26sql_query%3DSELECT%2B%252A%2BFROM%2B%2560note%2560%26message_to_show%3DThe%2Brow%2Bhas%2Bbeen%2Bdeleted%26goto%3Dtbl_sql.php%26token%3Dee2d4b54d1204adf52a94b92264ae27a&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
-    <hyperlink ref="N13" r:id="rId11" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=practicalgroup&amp;pos=0&amp;sql_query=SELECT+%2A+FROM+%60nphsemr%60.%60practicalgroup%60+WHERE+%60practicalGroupID%60+%3D+%27P01%27&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
-    <hyperlink ref="O13" r:id="rId12" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=scenario&amp;pos=0&amp;sql_query=SELECT+%2A+FROM+%60nphsemr%60.%60scenario%60+WHERE+%60scenarioID%60+%3D+%27SC1%27&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
-    <hyperlink ref="G14" r:id="rId13" display="http://localhost:55/phpmyadmin/tbl_change.php?db=nphsemr&amp;table=note&amp;where_clause=%60note%60.%60noteID%60+%3D+4&amp;clause_is_unique=1&amp;sql_query=SELECT+%2A+FROM+%60note%60&amp;goto=sql.php&amp;default_action=update&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
-    <hyperlink ref="H14" r:id="rId14" display="http://localhost:55/phpmyadmin/tbl_change.php?db=nphsemr&amp;table=note&amp;where_clause=%60note%60.%60noteID%60+%3D+4&amp;clause_is_unique=1&amp;sql_query=SELECT+%2A+FROM+%60note%60&amp;goto=sql.php&amp;default_action=insert&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
-    <hyperlink ref="I14" r:id="rId15" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=note&amp;sql_query=DELETE+FROM+%60nphsemr%60.%60note%60+WHERE+%60note%60.%60noteID%60+%3D+4&amp;message_to_show=The+row+has+been+deleted&amp;goto=sql.php%3Fdb%3Dnphsemr%26table%3Dnote%26sql_query%3DSELECT%2B%252A%2BFROM%2B%2560note%2560%26message_to_show%3DThe%2Brow%2Bhas%2Bbeen%2Bdeleted%26goto%3Dtbl_sql.php%26token%3Dee2d4b54d1204adf52a94b92264ae27a&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
-    <hyperlink ref="N14" r:id="rId16" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=practicalgroup&amp;pos=0&amp;sql_query=SELECT+%2A+FROM+%60nphsemr%60.%60practicalgroup%60+WHERE+%60practicalGroupID%60+%3D+%27P01%27&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
-    <hyperlink ref="O14" r:id="rId17" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=scenario&amp;pos=0&amp;sql_query=SELECT+%2A+FROM+%60nphsemr%60.%60scenario%60+WHERE+%60scenarioID%60+%3D+%27SC1%27&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
-    <hyperlink ref="G15" r:id="rId18" display="http://localhost:55/phpmyadmin/tbl_change.php?db=nphsemr&amp;table=note&amp;where_clause=%60note%60.%60noteID%60+%3D+5&amp;clause_is_unique=1&amp;sql_query=SELECT+%2A+FROM+%60note%60&amp;goto=sql.php&amp;default_action=update&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
-    <hyperlink ref="H15" r:id="rId19" display="http://localhost:55/phpmyadmin/tbl_change.php?db=nphsemr&amp;table=note&amp;where_clause=%60note%60.%60noteID%60+%3D+5&amp;clause_is_unique=1&amp;sql_query=SELECT+%2A+FROM+%60note%60&amp;goto=sql.php&amp;default_action=insert&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
-    <hyperlink ref="I15" r:id="rId20" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=note&amp;sql_query=DELETE+FROM+%60nphsemr%60.%60note%60+WHERE+%60note%60.%60noteID%60+%3D+5&amp;message_to_show=The+row+has+been+deleted&amp;goto=sql.php%3Fdb%3Dnphsemr%26table%3Dnote%26sql_query%3DSELECT%2B%252A%2BFROM%2B%2560note%2560%26message_to_show%3DThe%2Brow%2Bhas%2Bbeen%2Bdeleted%26goto%3Dtbl_sql.php%26token%3Dee2d4b54d1204adf52a94b92264ae27a&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
-    <hyperlink ref="N15" r:id="rId21" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=practicalgroup&amp;pos=0&amp;sql_query=SELECT+%2A+FROM+%60nphsemr%60.%60practicalgroup%60+WHERE+%60practicalGroupID%60+%3D+%27P01%27&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
-    <hyperlink ref="O15" r:id="rId22" display="http://localhost:55/phpmyadmin/sql.php?db=nphsemr&amp;table=scenario&amp;pos=0&amp;sql_query=SELECT+%2A+FROM+%60nphsemr%60.%60scenario%60+WHERE+%60scenarioID%60+%3D+%27SC4%27&amp;token=ee2d4b54d1204adf52a94b92264ae27a"/>
+    <hyperlink ref="D8" r:id="rId1" display="http://hsemr-wpinapp.rhcloud.com/hsemr/createScenario.jsphttp://hsemr-wpinapp.rhcloud.com/hsemr/editScenario.jsp"/>
+    <hyperlink ref="D9" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Submitted metrics for iteration 12
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v2.xlsx
+++ b/Documents/Project Management/Metrics/Bug Metrics/Bug Metrics v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7650" tabRatio="722" firstSheet="7" activeTab="11"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7650" tabRatio="722" firstSheet="7" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 1" sheetId="3" r:id="rId1"/>
@@ -17,15 +17,17 @@
     <sheet name="Iteration 8" sheetId="13" r:id="rId8"/>
     <sheet name="Iteration 9" sheetId="14" r:id="rId9"/>
     <sheet name="Iteration 10" sheetId="15" r:id="rId10"/>
-    <sheet name="Guidelines for Bug Metrics" sheetId="2" r:id="rId11"/>
-    <sheet name="Overview" sheetId="12" r:id="rId12"/>
+    <sheet name="Iteration 11" sheetId="16" r:id="rId11"/>
+    <sheet name="Iteration 12" sheetId="17" r:id="rId12"/>
+    <sheet name="Guidelines for Bug Metrics" sheetId="2" r:id="rId13"/>
+    <sheet name="Overview" sheetId="12" r:id="rId14"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="232">
   <si>
     <t>S/N</t>
   </si>
@@ -649,6 +651,84 @@
   </si>
   <si>
     <t>Change the div class so that the button expands the information</t>
+  </si>
+  <si>
+    <t>PDF Text Recog - Keywords</t>
+  </si>
+  <si>
+    <t>NPE for adding of keywords</t>
+  </si>
+  <si>
+    <t>FileNotFoundException, User Mapped File is opened</t>
+  </si>
+  <si>
+    <t>Check for NullPointerException</t>
+  </si>
+  <si>
+    <t>Catch fileNotFoundException and do not store files on the path, straight away delete it</t>
+  </si>
+  <si>
+    <t>Iteration 11 ( 09 March 2015 - 23 March 2015)</t>
+  </si>
+  <si>
+    <t>activateScenarioAdmin.jsp</t>
+  </si>
+  <si>
+    <t>activated case for lecturer box out of line</t>
+  </si>
+  <si>
+    <t>Activate Case</t>
+  </si>
+  <si>
+    <t>Deactivate Case</t>
+  </si>
+  <si>
+    <t>deactivateScenarioAdmin.jsp</t>
+  </si>
+  <si>
+    <t>"Current documents" heading not aligned</t>
+  </si>
+  <si>
+    <t>"Next" button is above the medication table</t>
+  </si>
+  <si>
+    <t>viewReportDocument.jsp</t>
+  </si>
+  <si>
+    <t>viewMedication.jsp</t>
+  </si>
+  <si>
+    <t>View Reports</t>
+  </si>
+  <si>
+    <t>View Medication</t>
+  </si>
+  <si>
+    <t>Submit multidisciplinary textbox</t>
+  </si>
+  <si>
+    <t>Textbox does not start from first position</t>
+  </si>
+  <si>
+    <t>ViewPatientInformation</t>
+  </si>
+  <si>
+    <t>medication tab, the step 3 red color fonts should be bigger</t>
+  </si>
+  <si>
+    <t>ViewPatientInformation.jsp</t>
+  </si>
+  <si>
+    <t>Iteration 12 (24 March 2015 - 6 April 2015)</t>
+  </si>
+  <si>
+    <t>delete button for document is in green but delete button for report is in red. need to standardize</t>
+  </si>
+  <si>
+    <t>Create case</t>
+  </si>
+  <si>
+    <t>createScenario.jsp</t>
   </si>
 </sst>
 </file>
@@ -792,7 +872,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -1034,13 +1114,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1384,6 +1477,16 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1566,10 +1669,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Overview!$C$3:$C$12</c:f>
+              <c:f>Overview!$C$3:$C$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>9</c:v>
                 </c:pt>
@@ -1586,6 +1689,12 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
@@ -1677,10 +1786,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Overview!$D$3:$D$12</c:f>
+              <c:f>Overview!$D$3:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1710,6 +1819,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1886,8 +1998,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1355913136"/>
-        <c:axId val="-1355914224"/>
+        <c:axId val="-993308720"/>
+        <c:axId val="-993300016"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1991,10 +2103,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Overview!$F$3:$F$12</c:f>
+              <c:f>Overview!$F$3:$F$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>14</c:v>
                 </c:pt>
@@ -2025,6 +2137,12 @@
                 <c:pt idx="9">
                   <c:v>9</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2040,11 +2158,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1355913136"/>
-        <c:axId val="-1355914224"/>
+        <c:axId val="-993308720"/>
+        <c:axId val="-993300016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1355913136"/>
+        <c:axId val="-993308720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2123,7 +2241,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1355914224"/>
+        <c:crossAx val="-993300016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2131,7 +2249,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1355914224"/>
+        <c:axId val="-993300016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2168,7 +2286,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1355913136"/>
+        <c:crossAx val="-993308720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2297,7 +2415,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
@@ -2361,7 +2478,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -2406,7 +2522,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2427,10 +2542,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Overview!$E$3:$E$12</c:f>
+              <c:f>Overview!$E$3:$E$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2444,8 +2559,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1489620176"/>
-        <c:axId val="-1211929104"/>
+        <c:axId val="-993297840"/>
+        <c:axId val="-993306544"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2549,10 +2664,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Overview!$F$3:$F$12</c:f>
+              <c:f>Overview!$F$3:$F$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>14</c:v>
                 </c:pt>
@@ -2583,6 +2698,12 @@
                 <c:pt idx="9">
                   <c:v>9</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2598,11 +2719,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1489620176"/>
-        <c:axId val="-1211929104"/>
+        <c:axId val="-993297840"/>
+        <c:axId val="-993306544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1489620176"/>
+        <c:axId val="-993297840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2681,7 +2802,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1211929104"/>
+        <c:crossAx val="-993306544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2689,7 +2810,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1211929104"/>
+        <c:axId val="-993306544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2726,7 +2847,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1489620176"/>
+        <c:crossAx val="-993297840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3165,7 +3286,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L17"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -3189,28 +3310,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="122" t="s">
+      <c r="B2" s="126" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="123"/>
-      <c r="D2" s="123"/>
-      <c r="E2" s="123"/>
-      <c r="F2" s="123"/>
-      <c r="G2" s="123"/>
-      <c r="H2" s="123"/>
-      <c r="I2" s="123"/>
-      <c r="J2" s="123"/>
-      <c r="K2" s="123"/>
-      <c r="L2" s="124"/>
+      <c r="C2" s="127"/>
+      <c r="D2" s="127"/>
+      <c r="E2" s="127"/>
+      <c r="F2" s="127"/>
+      <c r="G2" s="127"/>
+      <c r="H2" s="127"/>
+      <c r="I2" s="127"/>
+      <c r="J2" s="127"/>
+      <c r="K2" s="127"/>
+      <c r="L2" s="128"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="126" t="s">
+      <c r="B4" s="130" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="126"/>
+      <c r="C4" s="130"/>
       <c r="D4" s="15">
         <f>SUM(G8:G17)</f>
         <v>14</v>
@@ -3219,30 +3340,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="125" t="s">
+      <c r="G4" s="129" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="125"/>
-      <c r="I4" s="125"/>
-      <c r="J4" s="125"/>
-      <c r="K4" s="125"/>
-      <c r="L4" s="125"/>
+      <c r="H4" s="129"/>
+      <c r="I4" s="129"/>
+      <c r="J4" s="129"/>
+      <c r="K4" s="129"/>
+      <c r="L4" s="129"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="122" t="s">
+      <c r="B6" s="126" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="123"/>
-      <c r="G6" s="123"/>
-      <c r="H6" s="123"/>
-      <c r="I6" s="123"/>
-      <c r="J6" s="123"/>
-      <c r="K6" s="123"/>
-      <c r="L6" s="124"/>
+      <c r="C6" s="127"/>
+      <c r="D6" s="127"/>
+      <c r="E6" s="127"/>
+      <c r="F6" s="127"/>
+      <c r="G6" s="127"/>
+      <c r="H6" s="127"/>
+      <c r="I6" s="127"/>
+      <c r="J6" s="127"/>
+      <c r="K6" s="127"/>
+      <c r="L6" s="128"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="10" t="s">
@@ -3655,7 +3776,7 @@
   <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="I8" sqref="I8:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -3678,26 +3799,26 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="135" t="s">
+      <c r="B2" s="139" t="s">
         <v>200</v>
       </c>
-      <c r="C2" s="136"/>
-      <c r="D2" s="136"/>
-      <c r="E2" s="136"/>
-      <c r="F2" s="136"/>
-      <c r="G2" s="136"/>
-      <c r="H2" s="136"/>
-      <c r="I2" s="136"/>
-      <c r="J2" s="136"/>
-      <c r="K2" s="136"/>
-      <c r="L2" s="137"/>
+      <c r="C2" s="140"/>
+      <c r="D2" s="140"/>
+      <c r="E2" s="140"/>
+      <c r="F2" s="140"/>
+      <c r="G2" s="140"/>
+      <c r="H2" s="140"/>
+      <c r="I2" s="140"/>
+      <c r="J2" s="140"/>
+      <c r="K2" s="140"/>
+      <c r="L2" s="141"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="138" t="s">
+      <c r="B4" s="142" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="139"/>
+      <c r="C4" s="143"/>
       <c r="D4" s="44">
         <f>SUM(G8:G113)</f>
         <v>9</v>
@@ -3706,30 +3827,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="132" t="s">
+      <c r="G4" s="136" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="133"/>
-      <c r="I4" s="133"/>
-      <c r="J4" s="133"/>
-      <c r="K4" s="133"/>
-      <c r="L4" s="134"/>
+      <c r="H4" s="137"/>
+      <c r="I4" s="137"/>
+      <c r="J4" s="137"/>
+      <c r="K4" s="137"/>
+      <c r="L4" s="138"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="135" t="s">
+      <c r="B6" s="139" t="s">
         <v>173</v>
       </c>
-      <c r="C6" s="136"/>
-      <c r="D6" s="136"/>
-      <c r="E6" s="136"/>
-      <c r="F6" s="136"/>
-      <c r="G6" s="136"/>
-      <c r="H6" s="136"/>
-      <c r="I6" s="136"/>
-      <c r="J6" s="136"/>
-      <c r="K6" s="136"/>
-      <c r="L6" s="137"/>
+      <c r="C6" s="140"/>
+      <c r="D6" s="140"/>
+      <c r="E6" s="140"/>
+      <c r="F6" s="140"/>
+      <c r="G6" s="140"/>
+      <c r="H6" s="140"/>
+      <c r="I6" s="140"/>
+      <c r="J6" s="140"/>
+      <c r="K6" s="140"/>
+      <c r="L6" s="141"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="112" t="s">
@@ -4058,6 +4179,708 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q20"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="95"/>
+    <col min="2" max="2" width="4.42578125" style="95" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" style="95" customWidth="1"/>
+    <col min="4" max="4" width="42.5703125" style="95" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="95" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="95" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" style="95" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" style="95" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="95" customWidth="1"/>
+    <col min="10" max="10" width="31" style="95" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" style="95" customWidth="1"/>
+    <col min="12" max="12" width="14" style="95" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" style="95" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="95"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="139" t="s">
+        <v>211</v>
+      </c>
+      <c r="C2" s="140"/>
+      <c r="D2" s="140"/>
+      <c r="E2" s="140"/>
+      <c r="F2" s="140"/>
+      <c r="G2" s="140"/>
+      <c r="H2" s="140"/>
+      <c r="I2" s="140"/>
+      <c r="J2" s="140"/>
+      <c r="K2" s="140"/>
+      <c r="L2" s="141"/>
+    </row>
+    <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="142" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="143"/>
+      <c r="D4" s="44">
+        <v>13</v>
+      </c>
+      <c r="E4" s="45"/>
+      <c r="F4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="136" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="137"/>
+      <c r="I4" s="137"/>
+      <c r="J4" s="137"/>
+      <c r="K4" s="137"/>
+      <c r="L4" s="138"/>
+    </row>
+    <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="139" t="s">
+        <v>173</v>
+      </c>
+      <c r="C6" s="140"/>
+      <c r="D6" s="140"/>
+      <c r="E6" s="140"/>
+      <c r="F6" s="140"/>
+      <c r="G6" s="140"/>
+      <c r="H6" s="140"/>
+      <c r="I6" s="140"/>
+      <c r="J6" s="140"/>
+      <c r="K6" s="140"/>
+      <c r="L6" s="141"/>
+    </row>
+    <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="122" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="122" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="122" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="122" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="122" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="115"/>
+      <c r="B8" s="104">
+        <v>1</v>
+      </c>
+      <c r="C8" s="104" t="s">
+        <v>206</v>
+      </c>
+      <c r="D8" s="104" t="s">
+        <v>206</v>
+      </c>
+      <c r="E8" s="104" t="s">
+        <v>207</v>
+      </c>
+      <c r="F8" s="107">
+        <v>42070</v>
+      </c>
+      <c r="G8" s="104">
+        <v>5</v>
+      </c>
+      <c r="H8" s="100" t="str">
+        <f>IFERROR(VLOOKUP(G8,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v xml:space="preserve">High Impact </v>
+      </c>
+      <c r="I8" s="104" t="s">
+        <v>57</v>
+      </c>
+      <c r="J8" s="104" t="s">
+        <v>209</v>
+      </c>
+      <c r="K8" s="101" t="s">
+        <v>55</v>
+      </c>
+      <c r="L8" s="101">
+        <v>42146</v>
+      </c>
+      <c r="M8" s="115"/>
+      <c r="N8" s="115"/>
+      <c r="O8" s="115"/>
+      <c r="P8" s="115"/>
+      <c r="Q8" s="115"/>
+    </row>
+    <row r="9" spans="1:17" ht="66.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="115"/>
+      <c r="B9" s="104">
+        <v>2</v>
+      </c>
+      <c r="C9" s="104" t="s">
+        <v>206</v>
+      </c>
+      <c r="D9" s="104" t="s">
+        <v>206</v>
+      </c>
+      <c r="E9" s="107" t="s">
+        <v>208</v>
+      </c>
+      <c r="F9" s="107">
+        <v>42070</v>
+      </c>
+      <c r="G9" s="104">
+        <v>5</v>
+      </c>
+      <c r="H9" s="100" t="str">
+        <f>IFERROR(VLOOKUP(G9,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v xml:space="preserve">High Impact </v>
+      </c>
+      <c r="I9" s="104" t="s">
+        <v>57</v>
+      </c>
+      <c r="J9" s="104" t="s">
+        <v>210</v>
+      </c>
+      <c r="K9" s="104" t="s">
+        <v>55</v>
+      </c>
+      <c r="L9" s="101">
+        <v>42146</v>
+      </c>
+      <c r="M9" s="115"/>
+      <c r="N9" s="115"/>
+      <c r="O9" s="115"/>
+      <c r="P9" s="115"/>
+      <c r="Q9" s="115"/>
+    </row>
+    <row r="10" spans="1:17" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="115"/>
+      <c r="B10" s="100">
+        <v>3</v>
+      </c>
+      <c r="C10" s="100" t="s">
+        <v>214</v>
+      </c>
+      <c r="D10" s="100" t="s">
+        <v>212</v>
+      </c>
+      <c r="E10" s="107" t="s">
+        <v>213</v>
+      </c>
+      <c r="F10" s="107">
+        <v>42070</v>
+      </c>
+      <c r="G10" s="100">
+        <v>1</v>
+      </c>
+      <c r="H10" s="100" t="str">
+        <f>IFERROR(VLOOKUP(G10,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v>Low Impact</v>
+      </c>
+      <c r="I10" s="104" t="s">
+        <v>57</v>
+      </c>
+      <c r="J10" s="100"/>
+      <c r="K10" s="100" t="s">
+        <v>182</v>
+      </c>
+      <c r="L10" s="107">
+        <v>42073</v>
+      </c>
+      <c r="M10" s="115"/>
+      <c r="N10" s="115"/>
+      <c r="O10" s="115"/>
+      <c r="P10" s="115"/>
+      <c r="Q10" s="115"/>
+    </row>
+    <row r="11" spans="1:17" s="63" customFormat="1" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="64"/>
+      <c r="B11" s="100">
+        <v>4</v>
+      </c>
+      <c r="C11" s="100" t="s">
+        <v>215</v>
+      </c>
+      <c r="D11" s="100" t="s">
+        <v>216</v>
+      </c>
+      <c r="E11" s="107" t="s">
+        <v>213</v>
+      </c>
+      <c r="F11" s="107">
+        <v>42070</v>
+      </c>
+      <c r="G11" s="100">
+        <v>1</v>
+      </c>
+      <c r="H11" s="100" t="str">
+        <f>IFERROR(VLOOKUP(G11,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v>Low Impact</v>
+      </c>
+      <c r="I11" s="104" t="s">
+        <v>57</v>
+      </c>
+      <c r="J11" s="100"/>
+      <c r="K11" s="100" t="s">
+        <v>182</v>
+      </c>
+      <c r="L11" s="107">
+        <v>42073</v>
+      </c>
+      <c r="M11" s="64"/>
+      <c r="N11" s="64"/>
+      <c r="O11" s="64"/>
+      <c r="P11" s="64"/>
+      <c r="Q11" s="64"/>
+    </row>
+    <row r="12" spans="1:17" s="63" customFormat="1" ht="83.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="64"/>
+      <c r="B12" s="100">
+        <v>5</v>
+      </c>
+      <c r="C12" s="100" t="s">
+        <v>230</v>
+      </c>
+      <c r="D12" s="100" t="s">
+        <v>231</v>
+      </c>
+      <c r="E12" s="107" t="s">
+        <v>229</v>
+      </c>
+      <c r="F12" s="107">
+        <v>42070</v>
+      </c>
+      <c r="G12" s="100">
+        <v>1</v>
+      </c>
+      <c r="H12" s="100" t="str">
+        <f>IFERROR(VLOOKUP(G12,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v>Low Impact</v>
+      </c>
+      <c r="I12" s="104" t="s">
+        <v>57</v>
+      </c>
+      <c r="J12" s="100"/>
+      <c r="K12" s="100" t="s">
+        <v>182</v>
+      </c>
+      <c r="L12" s="107">
+        <v>42073</v>
+      </c>
+      <c r="M12" s="64"/>
+      <c r="N12" s="64"/>
+      <c r="O12" s="64"/>
+      <c r="P12" s="64"/>
+      <c r="Q12" s="64"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B13" s="115"/>
+      <c r="C13" s="115"/>
+      <c r="D13" s="115"/>
+      <c r="E13" s="115"/>
+      <c r="F13" s="115"/>
+      <c r="G13" s="115"/>
+      <c r="H13" s="51" t="str">
+        <f>IFERROR(VLOOKUP(G13,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v/>
+      </c>
+      <c r="I13" s="115"/>
+      <c r="J13" s="115"/>
+      <c r="K13" s="115"/>
+      <c r="L13" s="115"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H14" s="51" t="str">
+        <f>IFERROR(VLOOKUP(G14,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H15" s="51" t="str">
+        <f>IFERROR(VLOOKUP(G15,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H16" s="51" t="str">
+        <f>IFERROR(VLOOKUP(G16,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H17" s="51" t="str">
+        <f>IFERROR(VLOOKUP(G17,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H18" s="97"/>
+    </row>
+    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H19" s="97"/>
+    </row>
+    <row r="20" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H20" s="97"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="G4:L4"/>
+    <mergeCell ref="B6:L6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P21"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="95"/>
+    <col min="2" max="2" width="4.42578125" style="95" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" style="95" customWidth="1"/>
+    <col min="4" max="4" width="42.5703125" style="95" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="95" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="95" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" style="95" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" style="95" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="95" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" style="95" customWidth="1"/>
+    <col min="11" max="11" width="14" style="95" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" style="95" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="95"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="139" t="s">
+        <v>228</v>
+      </c>
+      <c r="C2" s="140"/>
+      <c r="D2" s="140"/>
+      <c r="E2" s="140"/>
+      <c r="F2" s="140"/>
+      <c r="G2" s="140"/>
+      <c r="H2" s="140"/>
+      <c r="I2" s="140"/>
+      <c r="J2" s="140"/>
+      <c r="K2" s="141"/>
+    </row>
+    <row r="3" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:16" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="142" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="143"/>
+      <c r="D4" s="44">
+        <v>4</v>
+      </c>
+      <c r="E4" s="45"/>
+      <c r="F4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="136" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="137"/>
+      <c r="I4" s="137"/>
+      <c r="J4" s="137"/>
+      <c r="K4" s="138"/>
+    </row>
+    <row r="5" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="139" t="s">
+        <v>173</v>
+      </c>
+      <c r="C6" s="140"/>
+      <c r="D6" s="140"/>
+      <c r="E6" s="140"/>
+      <c r="F6" s="140"/>
+      <c r="G6" s="140"/>
+      <c r="H6" s="140"/>
+      <c r="I6" s="140"/>
+      <c r="J6" s="140"/>
+      <c r="K6" s="141"/>
+    </row>
+    <row r="7" spans="1:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="122" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="122" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="122" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="122" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="122" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="115"/>
+      <c r="B8" s="104">
+        <v>1</v>
+      </c>
+      <c r="C8" s="104" t="s">
+        <v>221</v>
+      </c>
+      <c r="D8" s="124" t="s">
+        <v>219</v>
+      </c>
+      <c r="E8" s="124" t="s">
+        <v>217</v>
+      </c>
+      <c r="F8" s="107">
+        <v>42096</v>
+      </c>
+      <c r="G8" s="104">
+        <v>5</v>
+      </c>
+      <c r="H8" s="100" t="str">
+        <f>IFERROR(VLOOKUP(G8,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v xml:space="preserve">High Impact </v>
+      </c>
+      <c r="I8" s="104" t="s">
+        <v>57</v>
+      </c>
+      <c r="J8" s="100" t="s">
+        <v>182</v>
+      </c>
+      <c r="K8" s="101">
+        <v>42099</v>
+      </c>
+      <c r="L8" s="115"/>
+      <c r="M8" s="115"/>
+      <c r="N8" s="115"/>
+      <c r="O8" s="115"/>
+      <c r="P8" s="115"/>
+    </row>
+    <row r="9" spans="1:16" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="115"/>
+      <c r="B9" s="104">
+        <v>2</v>
+      </c>
+      <c r="C9" s="104" t="s">
+        <v>222</v>
+      </c>
+      <c r="D9" s="125" t="s">
+        <v>220</v>
+      </c>
+      <c r="E9" s="125" t="s">
+        <v>218</v>
+      </c>
+      <c r="F9" s="107">
+        <v>42096</v>
+      </c>
+      <c r="G9" s="104">
+        <v>1</v>
+      </c>
+      <c r="H9" s="100" t="str">
+        <f>IFERROR(VLOOKUP(G9,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v>Low Impact</v>
+      </c>
+      <c r="I9" s="104" t="s">
+        <v>57</v>
+      </c>
+      <c r="J9" s="100" t="s">
+        <v>182</v>
+      </c>
+      <c r="K9" s="101">
+        <v>42099</v>
+      </c>
+      <c r="L9" s="115"/>
+      <c r="M9" s="115"/>
+      <c r="N9" s="115"/>
+      <c r="O9" s="115"/>
+      <c r="P9" s="115"/>
+    </row>
+    <row r="10" spans="1:16" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="115"/>
+      <c r="B10" s="100">
+        <v>3</v>
+      </c>
+      <c r="C10" s="123" t="s">
+        <v>223</v>
+      </c>
+      <c r="D10" s="124" t="s">
+        <v>227</v>
+      </c>
+      <c r="E10" s="100" t="s">
+        <v>224</v>
+      </c>
+      <c r="F10" s="107">
+        <v>42096</v>
+      </c>
+      <c r="G10" s="100">
+        <v>1</v>
+      </c>
+      <c r="H10" s="100" t="str">
+        <f>IFERROR(VLOOKUP(G10,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v>Low Impact</v>
+      </c>
+      <c r="I10" s="104" t="s">
+        <v>57</v>
+      </c>
+      <c r="J10" s="100" t="s">
+        <v>182</v>
+      </c>
+      <c r="K10" s="101">
+        <v>42099</v>
+      </c>
+      <c r="L10" s="115"/>
+      <c r="M10" s="115"/>
+      <c r="N10" s="115"/>
+      <c r="O10" s="115"/>
+      <c r="P10" s="115"/>
+    </row>
+    <row r="11" spans="1:16" s="63" customFormat="1" ht="41.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="64"/>
+      <c r="B11" s="100">
+        <v>4</v>
+      </c>
+      <c r="C11" s="100" t="s">
+        <v>225</v>
+      </c>
+      <c r="D11" s="124" t="s">
+        <v>227</v>
+      </c>
+      <c r="E11" s="100" t="s">
+        <v>226</v>
+      </c>
+      <c r="F11" s="107">
+        <v>42096</v>
+      </c>
+      <c r="G11" s="100">
+        <v>1</v>
+      </c>
+      <c r="H11" s="100" t="str">
+        <f>IFERROR(VLOOKUP(G11,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v>Low Impact</v>
+      </c>
+      <c r="I11" s="104" t="s">
+        <v>57</v>
+      </c>
+      <c r="J11" s="100" t="s">
+        <v>182</v>
+      </c>
+      <c r="K11" s="101">
+        <v>42099</v>
+      </c>
+      <c r="L11" s="64"/>
+      <c r="M11" s="64"/>
+      <c r="N11" s="64"/>
+      <c r="O11" s="64"/>
+      <c r="P11" s="64"/>
+    </row>
+    <row r="12" spans="1:16" s="63" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="95"/>
+      <c r="B12" s="95"/>
+      <c r="C12" s="95"/>
+      <c r="D12" s="95"/>
+      <c r="E12" s="95"/>
+      <c r="F12" s="95"/>
+      <c r="G12" s="95"/>
+      <c r="H12" s="95"/>
+      <c r="I12" s="95"/>
+      <c r="J12" s="95"/>
+      <c r="K12" s="95"/>
+      <c r="L12" s="95"/>
+      <c r="M12" s="64"/>
+      <c r="N12" s="64"/>
+      <c r="O12" s="64"/>
+      <c r="P12" s="64"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H15" s="51"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H16" s="51" t="str">
+        <f>IFERROR(VLOOKUP(G16,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H17" s="51" t="str">
+        <f>IFERROR(VLOOKUP(G17,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H18" s="51" t="str">
+        <f>IFERROR(VLOOKUP(G18,'Guidelines for Bug Metrics'!$B$3:$C$5,2), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H19" s="97"/>
+    </row>
+    <row r="20" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H20" s="97"/>
+    </row>
+    <row r="21" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H21" s="97"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="B6:K6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -4205,12 +5028,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F12"/>
+  <dimension ref="B2:F15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="X14" sqref="X14"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4388,6 +5211,43 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="110">
+        <v>11</v>
+      </c>
+      <c r="C13" s="78">
+        <v>3</v>
+      </c>
+      <c r="D13" s="110">
+        <v>2</v>
+      </c>
+      <c r="E13" s="78"/>
+      <c r="F13" s="78">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="110">
+        <v>12</v>
+      </c>
+      <c r="C14" s="78">
+        <v>4</v>
+      </c>
+      <c r="D14" s="78"/>
+      <c r="E14" s="78"/>
+      <c r="F14" s="78">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="110">
+        <v>13</v>
+      </c>
+      <c r="C15" s="78"/>
+      <c r="D15" s="78"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="78"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4423,28 +5283,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="122" t="s">
+      <c r="B2" s="126" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="123"/>
-      <c r="D2" s="123"/>
-      <c r="E2" s="123"/>
-      <c r="F2" s="123"/>
-      <c r="G2" s="123"/>
-      <c r="H2" s="123"/>
-      <c r="I2" s="123"/>
-      <c r="J2" s="123"/>
-      <c r="K2" s="123"/>
-      <c r="L2" s="124"/>
+      <c r="C2" s="127"/>
+      <c r="D2" s="127"/>
+      <c r="E2" s="127"/>
+      <c r="F2" s="127"/>
+      <c r="G2" s="127"/>
+      <c r="H2" s="127"/>
+      <c r="I2" s="127"/>
+      <c r="J2" s="127"/>
+      <c r="K2" s="127"/>
+      <c r="L2" s="128"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="126" t="s">
+      <c r="B4" s="130" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="126"/>
+      <c r="C4" s="130"/>
       <c r="D4" s="15">
         <f>SUM(G8:G10)</f>
         <v>11</v>
@@ -4453,30 +5313,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="125" t="s">
+      <c r="G4" s="129" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="125"/>
-      <c r="I4" s="125"/>
-      <c r="J4" s="125"/>
-      <c r="K4" s="125"/>
-      <c r="L4" s="125"/>
+      <c r="H4" s="129"/>
+      <c r="I4" s="129"/>
+      <c r="J4" s="129"/>
+      <c r="K4" s="129"/>
+      <c r="L4" s="129"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="122" t="s">
+      <c r="B6" s="126" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="123"/>
-      <c r="G6" s="123"/>
-      <c r="H6" s="123"/>
-      <c r="I6" s="123"/>
-      <c r="J6" s="123"/>
-      <c r="K6" s="123"/>
-      <c r="L6" s="124"/>
+      <c r="C6" s="127"/>
+      <c r="D6" s="127"/>
+      <c r="E6" s="127"/>
+      <c r="F6" s="127"/>
+      <c r="G6" s="127"/>
+      <c r="H6" s="127"/>
+      <c r="I6" s="127"/>
+      <c r="J6" s="127"/>
+      <c r="K6" s="127"/>
+      <c r="L6" s="128"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="17" t="s">
@@ -4773,28 +5633,28 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="122" t="s">
+      <c r="B2" s="126" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="123"/>
-      <c r="D2" s="123"/>
-      <c r="E2" s="123"/>
-      <c r="F2" s="123"/>
-      <c r="G2" s="123"/>
-      <c r="H2" s="123"/>
-      <c r="I2" s="123"/>
-      <c r="J2" s="123"/>
-      <c r="K2" s="123"/>
-      <c r="L2" s="124"/>
+      <c r="C2" s="127"/>
+      <c r="D2" s="127"/>
+      <c r="E2" s="127"/>
+      <c r="F2" s="127"/>
+      <c r="G2" s="127"/>
+      <c r="H2" s="127"/>
+      <c r="I2" s="127"/>
+      <c r="J2" s="127"/>
+      <c r="K2" s="127"/>
+      <c r="L2" s="128"/>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="2:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="126" t="s">
+      <c r="B4" s="130" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="126"/>
+      <c r="C4" s="130"/>
       <c r="D4" s="22">
         <f>SUM(G8:G10)</f>
         <v>15</v>
@@ -4803,30 +5663,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="125" t="s">
+      <c r="G4" s="129" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="125"/>
-      <c r="I4" s="125"/>
-      <c r="J4" s="125"/>
-      <c r="K4" s="125"/>
-      <c r="L4" s="125"/>
+      <c r="H4" s="129"/>
+      <c r="I4" s="129"/>
+      <c r="J4" s="129"/>
+      <c r="K4" s="129"/>
+      <c r="L4" s="129"/>
     </row>
     <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="122" t="s">
+      <c r="B6" s="126" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="123"/>
-      <c r="G6" s="123"/>
-      <c r="H6" s="123"/>
-      <c r="I6" s="123"/>
-      <c r="J6" s="123"/>
-      <c r="K6" s="123"/>
-      <c r="L6" s="124"/>
+      <c r="C6" s="127"/>
+      <c r="D6" s="127"/>
+      <c r="E6" s="127"/>
+      <c r="F6" s="127"/>
+      <c r="G6" s="127"/>
+      <c r="H6" s="127"/>
+      <c r="I6" s="127"/>
+      <c r="J6" s="127"/>
+      <c r="K6" s="127"/>
+      <c r="L6" s="128"/>
     </row>
     <row r="7" spans="2:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="27" t="s">
@@ -5124,28 +5984,28 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="127" t="s">
+      <c r="B2" s="131" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
-      <c r="F2" s="128"/>
-      <c r="G2" s="128"/>
-      <c r="H2" s="128"/>
-      <c r="I2" s="128"/>
-      <c r="J2" s="128"/>
-      <c r="K2" s="128"/>
-      <c r="L2" s="129"/>
+      <c r="C2" s="132"/>
+      <c r="D2" s="132"/>
+      <c r="E2" s="132"/>
+      <c r="F2" s="132"/>
+      <c r="G2" s="132"/>
+      <c r="H2" s="132"/>
+      <c r="I2" s="132"/>
+      <c r="J2" s="132"/>
+      <c r="K2" s="132"/>
+      <c r="L2" s="133"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="130" t="s">
+      <c r="B4" s="134" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="131"/>
+      <c r="C4" s="135"/>
       <c r="D4" s="22">
         <f>SUM(G8:G10)</f>
         <v>5</v>
@@ -5154,30 +6014,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="132" t="s">
+      <c r="G4" s="136" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="133"/>
-      <c r="I4" s="133"/>
-      <c r="J4" s="133"/>
-      <c r="K4" s="133"/>
-      <c r="L4" s="134"/>
+      <c r="H4" s="137"/>
+      <c r="I4" s="137"/>
+      <c r="J4" s="137"/>
+      <c r="K4" s="137"/>
+      <c r="L4" s="138"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="127" t="s">
+      <c r="B6" s="131" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="128"/>
-      <c r="D6" s="128"/>
-      <c r="E6" s="128"/>
-      <c r="F6" s="128"/>
-      <c r="G6" s="128"/>
-      <c r="H6" s="128"/>
-      <c r="I6" s="128"/>
-      <c r="J6" s="128"/>
-      <c r="K6" s="128"/>
-      <c r="L6" s="129"/>
+      <c r="C6" s="132"/>
+      <c r="D6" s="132"/>
+      <c r="E6" s="132"/>
+      <c r="F6" s="132"/>
+      <c r="G6" s="132"/>
+      <c r="H6" s="132"/>
+      <c r="I6" s="132"/>
+      <c r="J6" s="132"/>
+      <c r="K6" s="132"/>
+      <c r="L6" s="133"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="33" t="s">
@@ -5469,28 +6329,28 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="127" t="s">
+      <c r="B2" s="131" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
-      <c r="F2" s="128"/>
-      <c r="G2" s="128"/>
-      <c r="H2" s="128"/>
-      <c r="I2" s="128"/>
-      <c r="J2" s="128"/>
-      <c r="K2" s="128"/>
-      <c r="L2" s="129"/>
+      <c r="C2" s="132"/>
+      <c r="D2" s="132"/>
+      <c r="E2" s="132"/>
+      <c r="F2" s="132"/>
+      <c r="G2" s="132"/>
+      <c r="H2" s="132"/>
+      <c r="I2" s="132"/>
+      <c r="J2" s="132"/>
+      <c r="K2" s="132"/>
+      <c r="L2" s="133"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="21"/>
     </row>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="130" t="s">
+      <c r="B4" s="134" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="131"/>
+      <c r="C4" s="135"/>
       <c r="D4" s="22">
         <f>SUM(G8:G116)</f>
         <v>30</v>
@@ -5499,30 +6359,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="132" t="s">
+      <c r="G4" s="136" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="133"/>
-      <c r="I4" s="133"/>
-      <c r="J4" s="133"/>
-      <c r="K4" s="133"/>
-      <c r="L4" s="134"/>
+      <c r="H4" s="137"/>
+      <c r="I4" s="137"/>
+      <c r="J4" s="137"/>
+      <c r="K4" s="137"/>
+      <c r="L4" s="138"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="127" t="s">
+      <c r="B6" s="131" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="128"/>
-      <c r="D6" s="128"/>
-      <c r="E6" s="128"/>
-      <c r="F6" s="128"/>
-      <c r="G6" s="128"/>
-      <c r="H6" s="128"/>
-      <c r="I6" s="128"/>
-      <c r="J6" s="128"/>
-      <c r="K6" s="128"/>
-      <c r="L6" s="129"/>
+      <c r="C6" s="132"/>
+      <c r="D6" s="132"/>
+      <c r="E6" s="132"/>
+      <c r="F6" s="132"/>
+      <c r="G6" s="132"/>
+      <c r="H6" s="132"/>
+      <c r="I6" s="132"/>
+      <c r="J6" s="132"/>
+      <c r="K6" s="132"/>
+      <c r="L6" s="133"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="41" t="s">
@@ -5891,7 +6751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -5915,26 +6775,26 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="135" t="s">
+      <c r="B2" s="139" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="136"/>
-      <c r="D2" s="136"/>
-      <c r="E2" s="136"/>
-      <c r="F2" s="136"/>
-      <c r="G2" s="136"/>
-      <c r="H2" s="136"/>
-      <c r="I2" s="136"/>
-      <c r="J2" s="136"/>
-      <c r="K2" s="136"/>
-      <c r="L2" s="137"/>
+      <c r="C2" s="140"/>
+      <c r="D2" s="140"/>
+      <c r="E2" s="140"/>
+      <c r="F2" s="140"/>
+      <c r="G2" s="140"/>
+      <c r="H2" s="140"/>
+      <c r="I2" s="140"/>
+      <c r="J2" s="140"/>
+      <c r="K2" s="140"/>
+      <c r="L2" s="141"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="138" t="s">
+      <c r="B4" s="142" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="139"/>
+      <c r="C4" s="143"/>
       <c r="D4" s="44">
         <f>SUM(G8:G116)</f>
         <v>20</v>
@@ -5943,30 +6803,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="132" t="s">
+      <c r="G4" s="136" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="133"/>
-      <c r="I4" s="133"/>
-      <c r="J4" s="133"/>
-      <c r="K4" s="133"/>
-      <c r="L4" s="134"/>
+      <c r="H4" s="137"/>
+      <c r="I4" s="137"/>
+      <c r="J4" s="137"/>
+      <c r="K4" s="137"/>
+      <c r="L4" s="138"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="135" t="s">
+      <c r="B6" s="139" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="136"/>
-      <c r="D6" s="136"/>
-      <c r="E6" s="136"/>
-      <c r="F6" s="136"/>
-      <c r="G6" s="136"/>
-      <c r="H6" s="136"/>
-      <c r="I6" s="136"/>
-      <c r="J6" s="136"/>
-      <c r="K6" s="136"/>
-      <c r="L6" s="137"/>
+      <c r="C6" s="140"/>
+      <c r="D6" s="140"/>
+      <c r="E6" s="140"/>
+      <c r="F6" s="140"/>
+      <c r="G6" s="140"/>
+      <c r="H6" s="140"/>
+      <c r="I6" s="140"/>
+      <c r="J6" s="140"/>
+      <c r="K6" s="140"/>
+      <c r="L6" s="141"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="34" t="s">
@@ -6327,26 +7187,26 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="135" t="s">
+      <c r="B2" s="139" t="s">
         <v>171</v>
       </c>
-      <c r="C2" s="136"/>
-      <c r="D2" s="136"/>
-      <c r="E2" s="136"/>
-      <c r="F2" s="136"/>
-      <c r="G2" s="136"/>
-      <c r="H2" s="136"/>
-      <c r="I2" s="136"/>
-      <c r="J2" s="136"/>
-      <c r="K2" s="136"/>
-      <c r="L2" s="137"/>
+      <c r="C2" s="140"/>
+      <c r="D2" s="140"/>
+      <c r="E2" s="140"/>
+      <c r="F2" s="140"/>
+      <c r="G2" s="140"/>
+      <c r="H2" s="140"/>
+      <c r="I2" s="140"/>
+      <c r="J2" s="140"/>
+      <c r="K2" s="140"/>
+      <c r="L2" s="141"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="138" t="s">
+      <c r="B4" s="142" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="139"/>
+      <c r="C4" s="143"/>
       <c r="D4" s="44">
         <f>SUM(G8:G115)</f>
         <v>15</v>
@@ -6355,30 +7215,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="132" t="s">
+      <c r="G4" s="136" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="133"/>
-      <c r="I4" s="133"/>
-      <c r="J4" s="133"/>
-      <c r="K4" s="133"/>
-      <c r="L4" s="134"/>
+      <c r="H4" s="137"/>
+      <c r="I4" s="137"/>
+      <c r="J4" s="137"/>
+      <c r="K4" s="137"/>
+      <c r="L4" s="138"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="135" t="s">
+      <c r="B6" s="139" t="s">
         <v>172</v>
       </c>
-      <c r="C6" s="136"/>
-      <c r="D6" s="136"/>
-      <c r="E6" s="136"/>
-      <c r="F6" s="136"/>
-      <c r="G6" s="136"/>
-      <c r="H6" s="136"/>
-      <c r="I6" s="136"/>
-      <c r="J6" s="136"/>
-      <c r="K6" s="136"/>
-      <c r="L6" s="137"/>
+      <c r="C6" s="140"/>
+      <c r="D6" s="140"/>
+      <c r="E6" s="140"/>
+      <c r="F6" s="140"/>
+      <c r="G6" s="140"/>
+      <c r="H6" s="140"/>
+      <c r="I6" s="140"/>
+      <c r="J6" s="140"/>
+      <c r="K6" s="140"/>
+      <c r="L6" s="141"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="62" t="s">
@@ -6812,26 +7672,26 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="135" t="s">
+      <c r="B2" s="139" t="s">
         <v>142</v>
       </c>
-      <c r="C2" s="136"/>
-      <c r="D2" s="136"/>
-      <c r="E2" s="136"/>
-      <c r="F2" s="136"/>
-      <c r="G2" s="136"/>
-      <c r="H2" s="136"/>
-      <c r="I2" s="136"/>
-      <c r="J2" s="136"/>
-      <c r="K2" s="136"/>
-      <c r="L2" s="137"/>
+      <c r="C2" s="140"/>
+      <c r="D2" s="140"/>
+      <c r="E2" s="140"/>
+      <c r="F2" s="140"/>
+      <c r="G2" s="140"/>
+      <c r="H2" s="140"/>
+      <c r="I2" s="140"/>
+      <c r="J2" s="140"/>
+      <c r="K2" s="140"/>
+      <c r="L2" s="141"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="138" t="s">
+      <c r="B4" s="142" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="139"/>
+      <c r="C4" s="143"/>
       <c r="D4" s="44">
         <f>SUM(G8:G110)</f>
         <v>32</v>
@@ -6840,30 +7700,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="132" t="s">
+      <c r="G4" s="136" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="133"/>
-      <c r="I4" s="133"/>
-      <c r="J4" s="133"/>
-      <c r="K4" s="133"/>
-      <c r="L4" s="134"/>
+      <c r="H4" s="137"/>
+      <c r="I4" s="137"/>
+      <c r="J4" s="137"/>
+      <c r="K4" s="137"/>
+      <c r="L4" s="138"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="135" t="s">
+      <c r="B6" s="139" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="136"/>
-      <c r="D6" s="136"/>
-      <c r="E6" s="136"/>
-      <c r="F6" s="136"/>
-      <c r="G6" s="136"/>
-      <c r="H6" s="136"/>
-      <c r="I6" s="136"/>
-      <c r="J6" s="136"/>
-      <c r="K6" s="136"/>
-      <c r="L6" s="137"/>
+      <c r="C6" s="140"/>
+      <c r="D6" s="140"/>
+      <c r="E6" s="140"/>
+      <c r="F6" s="140"/>
+      <c r="G6" s="140"/>
+      <c r="H6" s="140"/>
+      <c r="I6" s="140"/>
+      <c r="J6" s="140"/>
+      <c r="K6" s="140"/>
+      <c r="L6" s="141"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="93" t="s">
@@ -7276,26 +8136,26 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="135" t="s">
+      <c r="B2" s="139" t="s">
         <v>173</v>
       </c>
-      <c r="C2" s="136"/>
-      <c r="D2" s="136"/>
-      <c r="E2" s="136"/>
-      <c r="F2" s="136"/>
-      <c r="G2" s="136"/>
-      <c r="H2" s="136"/>
-      <c r="I2" s="136"/>
-      <c r="J2" s="136"/>
-      <c r="K2" s="136"/>
-      <c r="L2" s="137"/>
+      <c r="C2" s="140"/>
+      <c r="D2" s="140"/>
+      <c r="E2" s="140"/>
+      <c r="F2" s="140"/>
+      <c r="G2" s="140"/>
+      <c r="H2" s="140"/>
+      <c r="I2" s="140"/>
+      <c r="J2" s="140"/>
+      <c r="K2" s="140"/>
+      <c r="L2" s="141"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="138" t="s">
+      <c r="B4" s="142" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="139"/>
+      <c r="C4" s="143"/>
       <c r="D4" s="44">
         <f>SUM(G8:G113)</f>
         <v>8</v>
@@ -7304,30 +8164,30 @@
       <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="132" t="s">
+      <c r="G4" s="136" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="133"/>
-      <c r="I4" s="133"/>
-      <c r="J4" s="133"/>
-      <c r="K4" s="133"/>
-      <c r="L4" s="134"/>
+      <c r="H4" s="137"/>
+      <c r="I4" s="137"/>
+      <c r="J4" s="137"/>
+      <c r="K4" s="137"/>
+      <c r="L4" s="138"/>
     </row>
     <row r="5" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="135" t="s">
+      <c r="B6" s="139" t="s">
         <v>173</v>
       </c>
-      <c r="C6" s="136"/>
-      <c r="D6" s="136"/>
-      <c r="E6" s="136"/>
-      <c r="F6" s="136"/>
-      <c r="G6" s="136"/>
-      <c r="H6" s="136"/>
-      <c r="I6" s="136"/>
-      <c r="J6" s="136"/>
-      <c r="K6" s="136"/>
-      <c r="L6" s="137"/>
+      <c r="C6" s="140"/>
+      <c r="D6" s="140"/>
+      <c r="E6" s="140"/>
+      <c r="F6" s="140"/>
+      <c r="G6" s="140"/>
+      <c r="H6" s="140"/>
+      <c r="I6" s="140"/>
+      <c r="J6" s="140"/>
+      <c r="K6" s="140"/>
+      <c r="L6" s="141"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="98" t="s">

</xml_diff>